<commit_message>
cuadrando aún el home
</commit_message>
<xml_diff>
--- a/Clasificación para videos.xlsx
+++ b/Clasificación para videos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Gustavo\breslev-beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A8CBE0-C2CD-4DAA-B063-2DFF9283FA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A931800B-A497-40EB-B992-2D20968CA429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{20913F44-B740-45FA-9CAF-61CDE707757B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{20913F44-B740-45FA-9CAF-61CDE707757B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Temas frecuentes</t>
   </si>
@@ -43,16 +43,147 @@
   </si>
   <si>
     <t>La princesa perdida</t>
+  </si>
+  <si>
+    <t>Biografía Rabi Natan</t>
+  </si>
+  <si>
+    <t>Biografía Rabi Natan, saborear Pesaj</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iAdV-n-tyDU</t>
+  </si>
+  <si>
+    <t>Biografía Rabi Natan, El orden de la Hitbodedut</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eOuNysBOzwE</t>
+  </si>
+  <si>
+    <t>Biografía Rabi Natan, El orden de la Hitbodedut 2</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PqthKaqYd-w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biografía de Rabi Natan, </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cc1R0mDPI9w</t>
+  </si>
+  <si>
+    <t>Biografía de Rabi Natan, El orden de la Hitbodedut 3</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nC440_B-bkg</t>
+  </si>
+  <si>
+    <t>Biografía de Rabi Natan</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=upd7PQ6cYzw</t>
+  </si>
+  <si>
+    <t>Biografía de Rabi Nata, El orden de la hitbodedut 4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5wUvlXwINrI</t>
+  </si>
+  <si>
+    <t>Biografía de Rabi Natan, El orden de la Hitbodedut 5</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=SQw9MolZbQA</t>
+  </si>
+  <si>
+    <t>Likutey Moharan, Biografia</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vPsj2pZW-n8</t>
+  </si>
+  <si>
+    <t>Ojala el Hombre rezará todo el día</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7UghkZF0qjw</t>
+  </si>
+  <si>
+    <t>Biografía de Rabi Natan de Breslev</t>
+  </si>
+  <si>
+    <t>Entre el Fuego y el agua</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8A0z-Gy9B2I</t>
+  </si>
+  <si>
+    <t>Alabanza al Tzadik</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ntouyRAIYgU</t>
+  </si>
+  <si>
+    <t>La Tzedaka para el Tzadik</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_daj4hLGgDk</t>
+  </si>
+  <si>
+    <t>Captar la luz infinita en la práctica</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z02i-ntSVwY</t>
+  </si>
+  <si>
+    <t>Mi fuego ardera hasta la llegada del mesias</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6wFV3aU38wg</t>
+  </si>
+  <si>
+    <t>El libro quemado y él ya es un tzadik</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Nrh5R9Et07k</t>
+  </si>
+  <si>
+    <t>Biografía de Rabí Natan de Breslev</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cabubXApF9Q</t>
+  </si>
+  <si>
+    <t>Uman</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NOaKEC0V37s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KhnAKgnbexQ</t>
+  </si>
+  <si>
+    <t>Mi Rosh HaShana</t>
+  </si>
+  <si>
+    <t>Lección 24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,13 +206,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,54 +531,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E191323-50BC-4615-B5BB-03A5D061E6D8}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <f>7.731*1.19</f>
-        <v>9.1998899999999999</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:B8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{285A951D-CAB5-4DC5-84BF-E13D4234CDA6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>